<commit_message>
add redondeo de primer idea seminario
</commit_message>
<xml_diff>
--- a/SEMINARIO/Propuesta de negocio/Formulario propuestas de negocios Franco Fazzito.xlsx
+++ b/SEMINARIO/Propuesta de negocio/Formulario propuestas de negocios Franco Fazzito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franco\Downloads\5TO\SEMINARIO\Propuesta de negocio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8728BCA-E1A1-40D0-8A1C-01E6AC8FB27D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4047950-681D-4204-BEA0-31BC60E27A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Caratula" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>Apellido y nombre del alumno:</t>
   </si>
@@ -252,63 +252,6 @@
        - A los clientes les resultará mucho más fácil indicar sus necesidades ya que
 solamente indicando el uso que le dará a la computadora y cuanto está dispuesto a gastar, se le creará el presupuesto correcto para este adaptándose a sus necesidades y su presupuesto.
 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Breve descripcion del negocio</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">: es una empresa que brinda soluciones de software </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>orientada</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> a la creacion y mantenimiento de servicios para tiendas de hardware.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Mercado Objetivo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>: El mercado objetivo definido es un mercado concentrado constituido por todos los locales de ventas de hardware ubicados en la ciudad de buenos aires debido a que en esta zona se radican la mayor cantidad de locales y también los de mayor envergadura tanto en volumen de ventas como de publico, ademas de que nuestros principales clientes se encuentran dentro de esta area geografica y tambien nos ayudara inicialmente a poder brindar soporte de forma eficiente, pero dado que nuestro servicio es online, en el futuro se puede expandir hacia el resto de la argentina sin ningún inconveniente y utilizando cambios de moneda correspondientes junto con los tipos habituales de uso para su armado se puede escalar hacia el resto del mundo.</t>
     </r>
   </si>
   <si>
@@ -662,6 +605,70 @@
       <t>:</t>
     </r>
   </si>
+  <si>
+    <t>Franco Fazzito</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Breve descripcion del negocio</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">: es una empresa que brinda soluciones de software </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>orientada</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> a la creacion y mantenimiento de servicios para tiendas de hardware, esto se lograra a traves de la comercializaron por suscripcion de su principal servicio el cual permite crear presupuestos de una computadora de forma automatica, asistir en el armado de la misma en caso de tener algun error o inconveniente asi como agregar trazabilidad en la entrega y reclamos junto con una correcta gestion de stock junto con notificaciones ante productos faltantes.</t>
+    </r>
+  </si>
+  <si>
+    <t>EMPRENDIMIENTO PERSONAL</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Mercado Objetivo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: El mercado objetivo definido es un mercado concentrado constituido por todos los locales de ventas de hardware ubicados en la ciudad de buenos aires debido a que en esta zona se radican la mayor cantidad de locales y también los de mayor envergadura tanto en volumen de ventas como de publico, ademas de que nuestros principales clientes se encuentran dentro de esta area geografica y tambien nos ayudara inicialmente a poder brindar soporte de forma eficiente, pero dado que nuestro servicio es online, en el futuro se puede expandir hacia el resto de la argentina sin ningún inconveniente y utilizando cambios de moneda correspondientes junto con los tipos habituales de uso para su armado se puede escalar hacia el resto del mundo.
+       - Dentro de esta area geografica se encuentran alrededor de 80 locales y en aumento, debido al gran aumento de los consumidores de las computadoras de este tipo quienes son jugadores profesionales de Esports - desarroladores - editores tanto de audio como de video que fue provocado por la pandemia, es por ello que se ve un mercado en pleno crecimiento y con unos consumidores cada vez exigentes.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -733,7 +740,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -756,6 +763,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF7CAAC"/>
         <bgColor rgb="FFF7CAAC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -932,7 +945,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -967,7 +980,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1024,10 +1037,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1036,8 +1049,21 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1257,7 +1283,7 @@
   <dimension ref="B1:K1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:I7"/>
+      <selection activeCell="C5" sqref="C5:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1305,7 +1331,9 @@
     </row>
     <row r="5" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="11"/>
-      <c r="C5" s="13"/>
+      <c r="C5" s="13" t="s">
+        <v>36</v>
+      </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -2425,10 +2453,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:G1000"/>
+  <dimension ref="B1:J1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:G47"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2439,21 +2467,26 @@
     <col min="8" max="26" width="9.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="17" t="s">
+    <row r="1" spans="2:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="19"/>
-    </row>
-    <row r="3" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="45" t="s">
-        <v>25</v>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="49"/>
+      <c r="J2" s="50"/>
+    </row>
+    <row r="3" spans="2:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="39" t="s">
+        <v>37</v>
       </c>
       <c r="C4" s="21"/>
       <c r="D4" s="21"/>
@@ -2461,7 +2494,7 @@
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
     </row>
-    <row r="5" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="23"/>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
@@ -2469,7 +2502,7 @@
       <c r="F5" s="24"/>
       <c r="G5" s="25"/>
     </row>
-    <row r="6" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="23"/>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
@@ -2477,7 +2510,7 @@
       <c r="F6" s="24"/>
       <c r="G6" s="25"/>
     </row>
-    <row r="7" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="23"/>
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
@@ -2485,7 +2518,7 @@
       <c r="F7" s="24"/>
       <c r="G7" s="25"/>
     </row>
-    <row r="8" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="23"/>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
@@ -2493,7 +2526,7 @@
       <c r="F8" s="24"/>
       <c r="G8" s="25"/>
     </row>
-    <row r="9" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="23"/>
       <c r="C9" s="24"/>
       <c r="D9" s="24"/>
@@ -2501,7 +2534,7 @@
       <c r="F9" s="24"/>
       <c r="G9" s="25"/>
     </row>
-    <row r="10" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="23"/>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
@@ -2509,7 +2542,7 @@
       <c r="F10" s="24"/>
       <c r="G10" s="25"/>
     </row>
-    <row r="11" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="23"/>
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
@@ -2517,7 +2550,7 @@
       <c r="F11" s="24"/>
       <c r="G11" s="25"/>
     </row>
-    <row r="12" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="23"/>
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
@@ -2525,7 +2558,7 @@
       <c r="F12" s="24"/>
       <c r="G12" s="25"/>
     </row>
-    <row r="13" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="23"/>
       <c r="C13" s="24"/>
       <c r="D13" s="24"/>
@@ -2533,7 +2566,7 @@
       <c r="F13" s="24"/>
       <c r="G13" s="25"/>
     </row>
-    <row r="14" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="23"/>
       <c r="C14" s="24"/>
       <c r="D14" s="24"/>
@@ -2541,7 +2574,7 @@
       <c r="F14" s="24"/>
       <c r="G14" s="25"/>
     </row>
-    <row r="15" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="26"/>
       <c r="C15" s="27"/>
       <c r="D15" s="27"/>
@@ -2549,9 +2582,9 @@
       <c r="F15" s="27"/>
       <c r="G15" s="28"/>
     </row>
-    <row r="16" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="45" t="s">
-        <v>26</v>
+    <row r="16" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="39" t="s">
+        <v>39</v>
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="21"/>
@@ -2655,7 +2688,7 @@
       <c r="F28" s="24"/>
       <c r="G28" s="25"/>
     </row>
-    <row r="29" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="26"/>
       <c r="C29" s="27"/>
       <c r="D29" s="27"/>
@@ -2664,7 +2697,7 @@
       <c r="G29" s="28"/>
     </row>
     <row r="30" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="45" t="s">
+      <c r="B30" s="20" t="s">
         <v>24</v>
       </c>
       <c r="C30" s="21"/>
@@ -2811,7 +2844,7 @@
     </row>
     <row r="48" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="30" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C48" s="31"/>
       <c r="D48" s="31"/>
@@ -3863,7 +3896,8 @@
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="H2:J2"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B4:G15"/>
     <mergeCell ref="B16:G29"/>
@@ -3879,7 +3913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:G1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A31" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B4" sqref="B4:G15"/>
     </sheetView>
   </sheetViews>
@@ -3904,7 +3938,7 @@
     </row>
     <row r="3" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="39" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="21"/>
@@ -4002,7 +4036,7 @@
       <c r="G15" s="28"/>
     </row>
     <row r="16" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="39" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="8"/>
@@ -4109,14 +4143,14 @@
     </row>
     <row r="29" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="12"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
       <c r="G29" s="16"/>
     </row>
     <row r="30" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="39" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="8"/>
@@ -4255,10 +4289,10 @@
     </row>
     <row r="47" spans="2:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B47" s="12"/>
-      <c r="C47" s="39"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="39"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="40"/>
       <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5356,8 +5390,8 @@
     </row>
     <row r="3" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="45" t="s">
-        <v>37</v>
+      <c r="B4" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="C4" s="21"/>
       <c r="D4" s="21"/>
@@ -5454,7 +5488,7 @@
       <c r="G15" s="28"/>
     </row>
     <row r="16" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="39" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="21"/>
@@ -5568,7 +5602,7 @@
       <c r="G29" s="28"/>
     </row>
     <row r="30" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="39" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="21"/>
@@ -6783,8 +6817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24:K31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6810,23 +6844,23 @@
     <row r="2" spans="2:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G3" s="22"/>
       <c r="H3" s="30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I3" s="22"/>
       <c r="J3" s="30" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K3" s="22"/>
     </row>
@@ -6942,13 +6976,13 @@
       <c r="B13" s="23"/>
       <c r="C13" s="25"/>
       <c r="D13" s="30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E13" s="22"/>
       <c r="F13" s="23"/>
       <c r="G13" s="25"/>
       <c r="H13" s="30" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I13" s="22"/>
       <c r="J13" s="23"/>
@@ -7076,14 +7110,14 @@
     </row>
     <row r="24" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
       <c r="F24" s="22"/>
       <c r="G24" s="30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H24" s="21"/>
       <c r="I24" s="21"/>
@@ -7560,7 +7594,7 @@
     <row r="65" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="67" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="40" t="s">
+      <c r="B67" s="45" t="s">
         <v>8</v>
       </c>
       <c r="C67" s="18"/>
@@ -8845,24 +8879,6 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="B3:C23"/>
-    <mergeCell ref="D3:E12"/>
-    <mergeCell ref="F3:G23"/>
-    <mergeCell ref="H3:I12"/>
-    <mergeCell ref="J3:K23"/>
-    <mergeCell ref="H13:I23"/>
-    <mergeCell ref="D13:E23"/>
-    <mergeCell ref="H36:I45"/>
-    <mergeCell ref="H46:I56"/>
-    <mergeCell ref="B24:F31"/>
-    <mergeCell ref="B36:C56"/>
-    <mergeCell ref="D36:E45"/>
-    <mergeCell ref="F36:G56"/>
-    <mergeCell ref="G24:K31"/>
-    <mergeCell ref="B34:K34"/>
-    <mergeCell ref="J36:K56"/>
-    <mergeCell ref="D46:E56"/>
     <mergeCell ref="B90:F97"/>
     <mergeCell ref="B57:F64"/>
     <mergeCell ref="G57:K64"/>
@@ -8875,6 +8891,24 @@
     <mergeCell ref="D69:E78"/>
     <mergeCell ref="D79:E89"/>
     <mergeCell ref="B69:C89"/>
+    <mergeCell ref="H36:I45"/>
+    <mergeCell ref="H46:I56"/>
+    <mergeCell ref="B24:F31"/>
+    <mergeCell ref="B36:C56"/>
+    <mergeCell ref="D36:E45"/>
+    <mergeCell ref="F36:G56"/>
+    <mergeCell ref="G24:K31"/>
+    <mergeCell ref="B34:K34"/>
+    <mergeCell ref="J36:K56"/>
+    <mergeCell ref="D46:E56"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B3:C23"/>
+    <mergeCell ref="D3:E12"/>
+    <mergeCell ref="F3:G23"/>
+    <mergeCell ref="H3:I12"/>
+    <mergeCell ref="J3:K23"/>
+    <mergeCell ref="H13:I23"/>
+    <mergeCell ref="D13:E23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape"/>

</xml_diff>

<commit_message>
add detalles de seminario
</commit_message>
<xml_diff>
--- a/SEMINARIO/Propuesta de negocio/Formulario propuestas de negocios Franco Fazzito.xlsx
+++ b/SEMINARIO/Propuesta de negocio/Formulario propuestas de negocios Franco Fazzito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franc\Downloads\5TO\SEMINARIO\Propuesta de negocio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595A606F-8CAE-48E2-B989-67520550C891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909B2CB1-9F8E-463D-B0CA-96D85D6803DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Caratula" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Apellido y nombre del alumno:</t>
-  </si>
-  <si>
-    <t>Año:    2020</t>
   </si>
   <si>
     <t xml:space="preserve">Nota: Las ideas de negocios aquí expuestas deben ser todas elegibles </t>
@@ -218,160 +215,10 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Relacion con los clientes:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>- Periodo de prueba del servicio y posterior calificacion.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Social media.
-- Soporte a usuarios.
-- Contacto formal via mail.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Propuesta de valor:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>- Llevar todo el complejo proceso de armado de una computadora a medida de punta a punta de forma trazable y digital de forma automatica resultando en un aumento en las ventas y fidelizacion del cliente para con la tienda.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Actividades Clave: 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>- Desarrollo del servicio y soporte.
-- Presentacion y entrega de prueba gratuita al cliente.
-- Evaluacion del producto.
-- Proceso de venta de suscripcion.
-- Marketing.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Asociados Clave: 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>- Tiendas de hardware.
-- Proovedores de pago en linea.
-- Webs de benchmarking para componentes, programas y juegos.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Recursos Clave: 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>- Equipo de trabajo multidisciplinario para el desarrollo.
-- Plataforma tecnologica.
-- Tiendas de hardware</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>EMPRENDIMIENTO PERSONAL</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Estructura de Costos: 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>- Infraestructura tecnologia.
-- Pago de recursos humanos.
-- Marketing.</t>
-    </r>
-  </si>
-  <si>
     <t>Franco Fazzito</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Recursos Clave: 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>- Equipo de trabajo multidisciplinario para el desarrollo.
-- Plataforma tecnologica.
-- Pymes con busquedas abiertas.
-- Jovenes que quieran trabajar.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -429,309 +276,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Segmentos de clientes:
- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Tiendas de hardware</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">que:
-    - Tienen problemas de organizacion en sus procesos internos.
-     - Buscan un aumento en el numero de ventas.
-     - Buscan una opmimizacion en sus procesos internos.
-     - Buscan servicios de calidad
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Asociados Clave: 
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Empresas que buscan jovenes.
-- Jovenes quienes quieran insertarse al mercado laboral.
-- Recruiters de las empresas.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Actividades Clave:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>- Desarrollo del servicio y soporte.
-- Evaluacion del producto y de las busquedas.
-- Marketing.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Actividades Clave: 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Desarrollo del servicio y soporte.
-- Evaluacion del producto y de las casas elegidas.
-- Proceso de venta de la casa.
-- Marketing.
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Asociados Clave:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Constructoras.
-- Suministradores de materias primas.
-- Proveedores de mapas.
-- Proovedores de pago en linea.
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Estructura de Costos:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>- Infraestructura tecnologia.
-- Pago de recursos humanos.
-- Pago hacia la constructora.
-- Marketing.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Fuente de Ingresos:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>- Cobro de comisión por la reservacion de la propiedad.
-- Ganancia por venta de la vivienda.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Fuente de Ingresos:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Pago a traves de suscripcion mensual o anual.
-- Versionado de pago en base al tamaño de la tienda.
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Recursos Clave:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Equipo de trabajo multidisciplinario para el desarrollo.
-- Plataforma tecnologica.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Lotes en venta para la construccion.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Propuesta de valor: 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>- Generar no solo un impacto economico sino tambien medioambiental y social ya que buscamos acercar casas sustentables con el medio ambiente y acordes a la necesidad de nuestro cliente, generando asi un modelo de triple impacto.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Relacion con los clientes: 
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Social media
-- Soporte a usuarios y empresas</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Relacion con los clientes:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>- Social media.
-- Soporte a usuarios y constructora.
-- Contacto formal via mail.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Segmentos de clientes:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Usuarios que:
-   - Buscan una vivienda mas sustentable con el ambiente.
-   - Buscan una inversion sostenible en el tiempo.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">   - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Buscan una vivienda a un mejor precio</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Canales:
 </t>
     </r>
@@ -778,8 +322,11 @@
     </r>
   </si>
   <si>
+    <t>Año:    2022</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Propuesta de valor: 
+      <t xml:space="preserve">Relacion con los clientes: 
 - </t>
     </r>
     <r>
@@ -789,26 +336,9 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Creacion de una plataforma de busqueda de empleo orientada a los jovenes quienes no cuentan con trabajo o tengan poca experiencia laboral, ayudando a la</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>problematica argentina que hay sobre el desempleo entre los jovenes quienes no pueden insertarse en el mercado laboral</t>
+      <t>Social media 
+- Plataformas de videollamada.
+- Soporte a usuarios y empresas</t>
     </r>
     <r>
       <rPr>
@@ -833,8 +363,76 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>- Las pymes pagaran cierta comision por publicar la busqueda.
+      <t xml:space="preserve">- Pago a través de suscripción mensual o anual.
+- Versionado de pago en base al tamaño de la tienda.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fuente de Ingresos:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Cobro de comisión por la reservación de la propiedad.
+- Ganancia por venta de la vivienda.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fuente de Ingresos:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Las pymes pagaran cierta comisión por publicar la búsqueda.
 - Anuncios dentro del sitio web.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Estructura de Costos: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Infraestructura tecnología.
+- Pago de recursos humanos.
+- Marketing.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Estructura de Costos:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Infraestructura tecnología.
+- Pago de recursos humanos.
+- Pago hacia la constructora.
+- Marketing.</t>
     </r>
   </si>
   <si>
@@ -893,7 +491,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Busquen ampliar su busqueda laboral de forma digital.</t>
+      <t>Busquen ampliar su búsqueda laboral de forma digital.</t>
     </r>
     <r>
       <rPr>
@@ -934,6 +532,283 @@
         <family val="2"/>
       </rPr>
       <t>Quieran vender o patrocinar su producto a un sector joven.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Segmentos de clientes:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Usuarios que:
+   - Buscan una vivienda más sustentable con el ambiente.
+   - Buscan una inversión sostenible en el tiempo.
+   - Buscan una vivienda a un mejor precio.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Segmentos de clientes:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tiendas de hardware que:
+    - Tienen problemas de organización en sus procesos internos.
+     - Buscan un aumento en el número de ventas.
+     - Buscan una optimización en sus procesos internos.
+     - Buscan servicios de calidad</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Relacion con los clientes:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Periodo de prueba del servicio y posterior calificación.
+- Social media.
+- Soporte a usuarios.
+- Contacto formal vía mail.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Relacion con los clientes:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Social media.
+- Soporte a usuarios y constructora.
+- Contacto formal vía mail.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Propuesta de valor:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Llevar todo el complejo proceso de armado de una computadora a medida de punta a punta de forma trazable y digital de forma automática resultando en un aumento en las ventas y fidelización del cliente para con la tienda.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Propuesta de valor: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Generar no solo un impacto económico sino también medioambiental y social ya que buscamos acercar casas sustentables con el medio ambiente y acordes a la necesidad de nuestro cliente, generando así un modelo de triple impacto.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Propuesta de valor: 
+- Creación de una plataforma de búsqueda de empleo orientada a los jóvenes quienes no cuentan con trabajo o tengan poca experiencia laboral junto con el acceso de distintas clases en vivo para poder conseguirlo, ayudando a reducir el problema de desocupación juvenil.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Actividades Clave: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Desarrollo del servicio y soporte.
+- Presentación y entrega de prueba gratuita al cliente.
+- Evaluación del producto.
+- Proceso de venta de suscripción.
+- Marketing.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Actividades Clave: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Desarrollo del servicio y soporte.
+- Evaluación del producto y de las casas elegidas.
+- Proceso de venta de la casa.
+- Marketing.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Actividades Clave:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Desarrollo del servicio y soporte.
+- Evaluación del producto y de las búsquedas.
+- Contacto con las empresas interesadas.
+- Marketing.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Recursos Clave: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Equipo de trabajo multidisciplinario para el desarrollo.
+- Plataforma tecnológica.
+- Pymes con búsquedas abiertas.
+- Jóvenes que quieran trabajar.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Recursos Clave:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Equipo de trabajo multidisciplinario para el desarrollo.
+- Plataforma tecnológica.
+- Lotes en venta para la construcción.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Recursos Clave: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Equipo de trabajo multidisciplinario para el desarrollo.
+- Plataforma tecnológica.
+- Tiendas de hardware.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Asociados Clave: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Tiendas de hardware.
+- Proveedores de pago en línea.
+- Webs de benchmarking para componentes, programas y juegos.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Asociados Clave:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">- Constructoras.
+- Suministradores de materias primas.
+- Proveedores de mapas.
+- Proveedores de pago en línea.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Asociados Clave: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Empresas que buscan jóvenes.
+- Jóvenes quienes quieran insertarse al mercado laboral.
+- Recruiters de las empresas.</t>
     </r>
   </si>
 </sst>
@@ -1440,23 +1315,6 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
           <a:r>
             <a:rPr lang="es-AR" sz="1100">
               <a:solidFill>
@@ -1467,23 +1325,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>La</a:t>
+            <a:t>La empresa llamada FSolutions se dedica a la brindar soluciones de software orientado a los locales de venta de hardware que buscan resolver sus principales problemáticas. Es por ello por lo que desarrolla diferentes productos que permiten la digitalización y gestión eficiente de sus procesos para poder lograr tanto un aumento en las ventas y ganancias del local como brindar un mejor acceso a la tecnología a la sociedad.</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> empresa llamada FSolutions se dedica a la brindar soluciones de software orientado a los locales de venta de hardware que buscan resolver sus principales problematicas. Es por ello que desarrolla diferentes productos que permiten la digitalizacion y gestion eficiente de sus procesos para poder lograr tanto un aumento en las ventas y ganancias del local como brindar un mejor acceso a la tecnologia por parte de las personas.</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-AR">
-            <a:effectLst/>
-          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:endParaRPr lang="es-AR" sz="1100"/>
@@ -1553,23 +1396,6 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
           <a:r>
             <a:rPr lang="es-AR" sz="1100">
               <a:solidFill>
@@ -1580,10 +1406,12 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Nuestro mercado</a:t>
+            <a:t>Nuestro mercado objetivo son todos los locales de venta de hardware que busquen mejorar sus procesos a través de digitalización y automatización mejorando así sus ganancias y posicionamiento con respecto a la competencia.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0">
+            <a:rPr lang="es-AR" sz="1100">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -1592,29 +1420,12 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> objetivo son todos los locales de venta de hardware que busquen mejorar sus procesos a traves de digitilzacion y automatizacion mejorando asi sus ganancias y posicionamiento con respecto a la competencia.</a:t>
+            <a:t>En un principio para poder brindar un soporte correcto se concentrará en la ciudad de Buenos aires debido a que en esta zona se radican la mayor cantidad de locales y también los de mayor envergadura tanto en volumen de ventas como de público, además de que nuestros principales clientes se encuentran dentro de esta área geográfica pero dado que nuestro servicio es online, en el futuro se puede expandir hacia el resto del país.</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0">
+            <a:rPr lang="es-AR" sz="1100">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -1623,11 +1434,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>En un principio para poder brindar un soporte correcto se concentrara en la ciudad de buenos aires debido a que en esta zona se radican la mayor cantidad de locales y también los de mayor envergadura tanto en volumen de ventas como de publico, ademas de que nuestros principales clientes se encuentran dentro de esta area geografica pero dado que nuestro servicio es online, en el futuro se puede expandir hacia el resto del pais.</a:t>
+            <a:t>Actualmente la solución Mobile que proponemos se encuentra dentro de 6 locales en la ciudad de Buenos Aires y la expectativa a futuro es positiva ya que existen alrededor de 80 locales restantes solo en ciudad de Buenos Aires.</a:t>
           </a:r>
-          <a:endParaRPr lang="es-AR">
-            <a:effectLst/>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1695,42 +1503,86 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>Nuestra</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
-            <a:t> empresa ofrecera un servicio de gestion de armado de computadoras a medida, mediante el cual nuestro cliente pueda llevar todo el complejo proceso de armado de una computadora de punta a punta de forma trazable y digital, siendo este nuestro principal diferenciador con respecto a otros softwares de gestion no especializados, contando con la posibilidad de:</a:t>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Nuestra empresa ofrecerá un servicio de gestión de armado de computadoras a medida, mediante el cual nuestro cliente pueda llevar todo el complejo proceso de armado de una computadora de punta a punta de forma trazable y digital, siendo este nuestro principal diferenciador con respecto a otros softwares de gestión no especializados, contando con la posibilidad de:</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
-            <a:t>- Crear presupuestos de forma automatica en base al presupuesto y tipo de uso del cliente que se acerca a la tienda.</a:t>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- Crear presupuestos de forma automática en base al presupuesto y tipo de uso del cliente que se acerca a la tienda.</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
-            <a:t>- Asignacion automatica del armado de la computadora al empleado mas ocioso.</a:t>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- Asignación automática del armado de la computadora al empleado más ocioso.</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
-            <a:t>- Llevar trazabilidad de los procesos de armado y entrega asi como indicar los fallos que tuvieron durante estos y asignar de forma automatica su repuesto.</a:t>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- Llevar trazabilidad de los procesos de armado y entrega, así como indicar los fallos que tuvieron durante estos y asignar de forma automática su repuesto.</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>- Gestionar el stock de cada uno de los componentes junto con un sistema de notificaciones cada vez que cierto componente este en falta.</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
-            <a:t>De esta forma se automatizan los procesos mas complejos de los locales de venta logrando un aumento en la productividad de los empleados junto con una mejora en el proceso de venta debido al mejor entendimiento de las necesidades del cliente y sumado a una mejora del servicio post venta en caso de algun fallo.</a:t>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>De esta forma se automatizan los procesos más complejos de los locales de venta logrando un aumento en la productividad de los empleados junto con una mejora en el proceso de venta debido al mejor entendimiento de las necesidades del cliente y sumado a una mejora del servicio post venta en caso de algún fallo.</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1799,51 +1651,119 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>Se plantea</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
-            <a:t> una plataforma tanto web como mobile que cuente con los siguientes modulos:</a:t>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Se plantea una plataforma tanto web como Mobile que cuente con los siguientes módulos:</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" b="1"/>
+            <a:rPr lang="es-AR" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>- Creador de presupuesto: </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100"/>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>a través de este módulo se permitirá ingresar tanto la cantidad de dinero (como pueden ser 100000 pesos argentinos) como el tipo de uso (como pueden ser: ofimática, diseño en 3D, videojuegos o edición de video) y la plataforma le responderá con los presupuestos más acordes para el cliente.</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" b="1"/>
+            <a:rPr lang="es-AR" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>- Asistente de armado: </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>a través de este módulo el empleado armara la computadora y también podrán indicar los fallos que tuvieron durante su armado, de esta forma la plataforma le indicara un reemplazo equivalente en calidad y precio para el componente de hardware defectuoso, posteriormente la plataforma registrara la incompatibilidad o mal funcionamiento para poder hacer mejores y más acertados presupuestos a medida que se usa, ademas de ello cuando se crea un pedido se asigna de forma automatica a su empleado mas ocioso.</a:t>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>a través de este módulo el empleado armara la computadora y también podrán indicar los fallos que tuvieron durante su armado, de esta forma la plataforma le indicara un reemplazo equivalente en calidad y precio para el componente de hardware defectuoso, posteriormente la plataforma registrara la incompatibilidad o mal funcionamiento para poder hacer mejores y más acertados presupuestos a medida que se usa, además de ello cuando se crea un pedido se asigna de forma automática a su empleado más ocioso.</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" b="1"/>
+            <a:rPr lang="es-AR" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>- Asistente de entrega: </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>una vez entregada la computadora se registrará dentro de la aplicación y en caso de que el cliente presente algún fallo o mal funcionamiento se registrara también junto con una incompatibilidad una vez revisada e indicando de forma automatica un reemplazo equivalente en calidad y precio para el componente de hardware defectuoso.</a:t>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>una vez entregada la computadora se registrará dentro de la aplicación y en caso de que el cliente presente algún fallo o mal funcionamiento se registrara también junto con una incompatibilidad una vez revisada e indicando de forma automática un reemplazo equivalente en calidad y precio para el componente de hardware defectuoso.</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" b="1"/>
+            <a:rPr lang="es-AR" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>- Gestión de stock: </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100"/>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>a través de este módulo se gestionarán todas las entradas y salidas de componentes de dentro de las tiendas además de contar con un sistema de notificación para cuando el stock de algún producto se encuentre por debajo de cierto limite.</a:t>
           </a:r>
         </a:p>
@@ -1927,67 +1847,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>La empresa llamada FSolution se dedica a</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-AR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>la construccion y comercializacion de viviendas sustentables con un sistema de rapida</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> construccion </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-AR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>que aunque son mas caras que las viviendas</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> clasicas si se toma el ahorro a lo largo de su vida util hace que sean mejores financiaramente hablando que las primeras, de esta forma se consiguen viviendas mas amigables con el medio ambiente debido al menor consumo de energia junto con un menor tiempo de construccion.</a:t>
+            <a:t>La empresa llamada FSolutions se dedica a la construcción y comercialización de viviendas sustentables con un sistema de rápida construcción que, aunque son más caras que las viviendas clásicas si se toma el ahorro a lo largo de su vida útil hace que sean mejores financieramente hablando que las primeras, de esta forma se consiguen viviendas más amigables con el medio ambiente debido al menor consumo de energía junto con un menor tiempo de construcción.</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2056,21 +1916,33 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>Nuestro mercado objetivo son todas</a:t>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Nuestro mercado objetivo son todas aquellas familias y personas que buscan una vivienda donde vivir de una manera más sustentable sin pagar más por ello.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
-            <a:t> </a:t>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Luego de la pandemia se vio un aumento en la demanda de este tipo de viviendas sumado a un claro aumento de preocupación social por el medio ambiente (https://marcas.eleconomista.es/vivienda/noticias/10785298/09/20/El-Covid19-genera-mas-demanda-de-viviendas-sostenibles-y-saludables.html).</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>aquellas familias y personas que buscan una vivienda donde</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
-            <a:t> vivir de una manera mas sustentable sin pagar mas por ello.</a:t>
-          </a:r>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="es-AR" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -2139,62 +2011,145 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>Como servicio principal de nuestra empresa contamos con una plataforma (web y mobile), mediante la cual todos sus usuarios son capaces de realizar la</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
-            <a:t> reservacion y planificacion para la construccion de casas sustentables en base a sus necesidades, brindando asi el espacio perfecto para su presupuesto y necesidad habitacional.</a:t>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Como servicio principal de nuestra empresa contamos con una plataforma (web y Mobile), mediante la cual todos sus usuarios son capaces de realizar la reservación y planificación para la construcción de casas sustentables en base a sus necesidades, brindando así el espacio perfecto para su presupuesto y necesidad habitacional.</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
-            <a:t>Ademas brindamos un modelo de triple impacto que no solo aporta valor economico sino tambien ambiental y social:</a:t>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Además, brindamos un modelo de triple impacto que no solo aporta valor económico sino también ambiental y social:</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>- </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" b="1" baseline="0"/>
+            <a:rPr lang="es-AR" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>Social: </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>facilita el acceso a la vivienda propia acorde a las necesidades del cliente.</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>- </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" b="1" baseline="0"/>
-            <a:t>Economico: </a:t>
+            <a:rPr lang="es-AR" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Económico: </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
-            <a:t>si bien la construccion de este tipo de casas es mas cara, a lo largo de su vida util son mejores financieramente ya que el ahorro energetico que se produce al utilizar una de estas es mucho mayor ademas de poder cumplir con un proceso de fabricacion mas rapido.</a:t>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>si bien la construcción de este tipo de casas es más cara, a lo largo de su vida útil son mejores financieramente ya que el ahorro energético que se produce al utilizar una de estas es mucho mayor además de poder cumplir con un proceso de fabricación más rápido.</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>- </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" b="1" baseline="0"/>
+            <a:rPr lang="es-AR" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>Ambiental:  </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
-            <a:t>mejora en forma considerable el uso de energia resultando en una mejora para el medio ambiente.</a:t>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>mejora en forma considerable el uso de energía resultando en una mejora para el medio ambiente.</a:t>
           </a:r>
-          <a:endParaRPr lang="es-AR" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2262,14 +2217,17 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>Se plantea una plataforma tanto web como mobile</a:t>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Se plantea una plataforma tanto web como Mobile que permita a los usuarios realizar la reservación y planificación de la construcción de casas sustentable en base a sus necesidades es por ello por lo que planteamos que los usuarios puedan ingresar diversos filtros y presupuestos en base a sus necesidades y capacidad de compra para que nuestra plataforma pueda mostrarle la casa ideal para ellos, de esta forma se facilita la compra por parte del cliente abonando una reserva de esta.</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
-            <a:t> que permita a los usuarios realizar la reservacion y planificacion de la construccion de casas sustentable en base a sus necesidades es por ello que planteamos que los usuarios puedan ingresar diversos filtros y presupuestos en base a sus necesidades y capacidad de compra para que nuestra plataforma pueda mostrarle la casa ideal para ellos, de esta forma se facilita la compra por parte del cliente abonando una reserva de la misma.</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-AR" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2341,23 +2299,6 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
           <a:r>
             <a:rPr lang="es-AR" sz="1100">
               <a:solidFill>
@@ -2368,29 +2309,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>La empresa llamada FSolutions se dedica a la brindar soluciones de software orientado al mercado laboral.</a:t>
+            <a:t>La empresa llamada FSolutions se dedica a la brindar soluciones de software orientado al mercado laboral, con este fin realiza trabajos de investigación sobre la sociedad argentina, y desarrolla diferentes productos que busca que todos los argentinos puedan acceder a su primer trabajo, es por ello por lo que se busca lanzar una plataforma donde los jóvenes puedan conseguir su primer trabajo acercando más oportunidades a un sector que sufre de desempleo.</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> Con este fin realiza trabajos de investigación sobre la sociedad Argentina, y desarrolla diferentes productos que busca que todos los argentinos puedan acceder a su primer trabajo, es por ello que se busca lanzar una plataforma donde los jovenes puedan conseguir su primer trabajo acercando mas oportunidades a un sector que sufre de desempleo.</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-AR" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2458,14 +2378,17 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>Nuestro mercado objetivo son todos los jov</a:t>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Nuestro mercado objetivo son todos los jóvenes que no poseen trabajo o tengan una corta experiencia laboral y quisieran conseguir trabajo, por otro lado, también apuntamos a pymes que quieran contratar este talento joven.</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
-            <a:t>enes que no poseen trabajo o tengan una corta experiencia laboral y quisieran conseguir trabajo, por otro lado tambien apuntamos a pymes que quieran contratar este talento joven.</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-AR" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2542,10 +2465,12 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Nuestra</a:t>
+            <a:t>Nuestra empresa ofrecerá una plataforma mediante la cual los usuarios puedan postularse a distintos puestos jrs o sin experiencia previa que son publicados por diferentes pymes que también formaran parte de la plataforma, de esta forma se podría ayudar a la gran problemática argentina (la argentina es el país con mayor desempleo juvenil del cono sur) que hay sobre el desempleo entre los jóvenes quienes no pueden insertarse en el mercado laboral y de esta forma caen en trabajos precarios e irregulares.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0">
+            <a:rPr lang="es-AR" sz="1100">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -2554,13 +2479,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> empresa ofrecera una </a:t>
+            <a:t>Además de ello se dictarán distintas capacitaciones dentro de la plataforma para poder conseguir este primer trabajo dictada por recruiters profesionales.</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
-            <a:t>plataforma mediante la cual los usuarios puedan postularse a distintos puestos jrs o sin experiencia previa que son publicados por diferentes pymes que tambien formaran parte de la plataforma, de esta forma se podria ayudar a la gran problematica argentina (la argentina es el pais con mayor desempleo juvenil del cono sur) que hay sobre el desempleo entre los jovenes quienes no pueden insertarse en el mercado laboral y de esta forma caen en trabajos precarios e irregulares.</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-AR" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2628,24 +2548,58 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>Se plantea</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
-            <a:t> una plataforma web donde:</a:t>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Se plantea una plataforma web donde:</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
-            <a:t>- los jovenes puedan puedan ver las ofertas de empleo disponibles y poder filtrarlas como asi deseen y donde puedan visualizar las empresas mas convenientes acorde a sus estudios, cursos o pasantias realizadas.</a:t>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- los jóvenes puedan ver las ofertas de empleo disponibles y poder filtrarlas como así deseen y donde puedan visualizar las empresas más convenientes acorde a sus estudios, cursos o pasantías realizadas.</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
-            <a:t>- las pymes publiquen las busquedas abiertas que tienen en su empresa asi como ver los posibles empleados mas capaces para dicho puesto.</a:t>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- las pymes publiquen las búsquedas abiertas que tienen en su empresa, así como ver los posibles empleados más capaces para dicho puesto.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- Se cuente con un módulo de acceso a las capacitaciones en vivo a través de una plataforma externa.</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2856,7 +2810,7 @@
   <dimension ref="B1:K1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="C11" sqref="C11:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2905,7 +2859,7 @@
     <row r="5" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="11"/>
       <c r="C5" s="13" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -2929,7 +2883,7 @@
     <row r="7" spans="2:11" ht="84" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="11"/>
       <c r="C7" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -2976,7 +2930,7 @@
     <row r="11" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="11"/>
       <c r="C11" s="4" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -2989,7 +2943,7 @@
     <row r="12" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="11"/>
       <c r="C12" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -4028,8 +3982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:J1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView showGridLines="0" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4043,7 +3997,7 @@
     <row r="1" spans="2:10" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -4051,7 +4005,7 @@
       <c r="F2" s="30"/>
       <c r="G2" s="31"/>
       <c r="H2" s="26" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="I2" s="27"/>
       <c r="J2" s="28"/>
@@ -4059,7 +4013,7 @@
     <row r="3" spans="2:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
@@ -4157,7 +4111,7 @@
     </row>
     <row r="16" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="33"/>
       <c r="D16" s="33"/>
@@ -4271,7 +4225,7 @@
     </row>
     <row r="30" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C30" s="33"/>
       <c r="D30" s="33"/>
@@ -4417,7 +4371,7 @@
     </row>
     <row r="48" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C48" s="18"/>
       <c r="D48" s="18"/>
@@ -5487,7 +5441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:G1000"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:G2"/>
     </sheetView>
   </sheetViews>
@@ -5502,7 +5456,7 @@
     <row r="1" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="42" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="43"/>
       <c r="D2" s="43"/>
@@ -5513,7 +5467,7 @@
     <row r="3" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
@@ -5611,7 +5565,7 @@
     </row>
     <row r="16" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="33"/>
       <c r="D16" s="33"/>
@@ -5725,7 +5679,7 @@
     </row>
     <row r="30" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C30" s="33"/>
       <c r="D30" s="33"/>
@@ -5871,7 +5825,7 @@
     </row>
     <row r="48" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C48" s="33"/>
       <c r="D48" s="33"/>
@@ -6940,7 +6894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:G1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:G2"/>
     </sheetView>
   </sheetViews>
@@ -6955,7 +6909,7 @@
     <row r="1" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="47"/>
       <c r="D2" s="47"/>
@@ -6966,7 +6920,7 @@
     <row r="3" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
@@ -7064,7 +7018,7 @@
     </row>
     <row r="16" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -7178,7 +7132,7 @@
     </row>
     <row r="30" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -7324,7 +7278,7 @@
     </row>
     <row r="48" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
@@ -8393,8 +8347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36:K56"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69:E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8407,7 +8361,7 @@
   <sheetData>
     <row r="1" spans="2:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="54" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="55"/>
       <c r="D1" s="55"/>
@@ -8422,23 +8376,23 @@
     <row r="2" spans="2:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="45" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C3" s="34"/>
       <c r="D3" s="45" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="E3" s="34"/>
       <c r="F3" s="45" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="G3" s="34"/>
       <c r="H3" s="45" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="I3" s="34"/>
       <c r="J3" s="45" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K3" s="34"/>
     </row>
@@ -8554,13 +8508,13 @@
       <c r="B13" s="35"/>
       <c r="C13" s="37"/>
       <c r="D13" s="45" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="E13" s="34"/>
       <c r="F13" s="35"/>
       <c r="G13" s="37"/>
       <c r="H13" s="45" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I13" s="34"/>
       <c r="J13" s="35"/>
@@ -8688,14 +8642,14 @@
     </row>
     <row r="24" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="45" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C24" s="33"/>
       <c r="D24" s="33"/>
       <c r="E24" s="33"/>
       <c r="F24" s="34"/>
       <c r="G24" s="45" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="H24" s="33"/>
       <c r="I24" s="33"/>
@@ -8790,7 +8744,7 @@
     <row r="33" spans="2:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="2:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="50" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34" s="43"/>
       <c r="D34" s="43"/>
@@ -8805,23 +8759,23 @@
     <row r="35" spans="2:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="45" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C36" s="34"/>
       <c r="D36" s="45" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E36" s="34"/>
       <c r="F36" s="45" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G36" s="34"/>
       <c r="H36" s="45" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="I36" s="34"/>
       <c r="J36" s="45" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="K36" s="34"/>
     </row>
@@ -8937,13 +8891,13 @@
       <c r="B46" s="35"/>
       <c r="C46" s="37"/>
       <c r="D46" s="45" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E46" s="34"/>
       <c r="F46" s="35"/>
       <c r="G46" s="37"/>
       <c r="H46" s="45" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="I46" s="34"/>
       <c r="J46" s="35"/>
@@ -9071,14 +9025,14 @@
     </row>
     <row r="57" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="45" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C57" s="33"/>
       <c r="D57" s="33"/>
       <c r="E57" s="33"/>
       <c r="F57" s="34"/>
       <c r="G57" s="45" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="H57" s="33"/>
       <c r="I57" s="33"/>
@@ -9173,7 +9127,7 @@
     <row r="66" spans="2:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="67" spans="2:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B67" s="51" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C67" s="52"/>
       <c r="D67" s="52"/>
@@ -9188,23 +9142,23 @@
     <row r="68" spans="2:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="45" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C69" s="34"/>
       <c r="D69" s="45" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E69" s="34"/>
       <c r="F69" s="45" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G69" s="34"/>
       <c r="H69" s="45" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="I69" s="34"/>
       <c r="J69" s="45" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="K69" s="34"/>
     </row>
@@ -9320,13 +9274,13 @@
       <c r="B79" s="35"/>
       <c r="C79" s="37"/>
       <c r="D79" s="45" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="E79" s="34"/>
       <c r="F79" s="35"/>
       <c r="G79" s="37"/>
       <c r="H79" s="45" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="I79" s="34"/>
       <c r="J79" s="35"/>
@@ -9454,14 +9408,14 @@
     </row>
     <row r="90" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B90" s="45" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C90" s="33"/>
       <c r="D90" s="33"/>
       <c r="E90" s="33"/>
       <c r="F90" s="34"/>
       <c r="G90" s="45" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="H90" s="33"/>
       <c r="I90" s="33"/>

</xml_diff>